<commit_message>
marc ctf1 und ctf4
</commit_message>
<xml_diff>
--- a/challenges.xlsx
+++ b/challenges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\twine-ctf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\uni_master\twine-ctf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F166A-C530-49B8-9A6A-B653EA80900A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C43A95-2E98-48BA-B872-9D5E7925A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChallengesÜbersicht" sheetId="1" r:id="rId1"/>
@@ -644,18 +644,18 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -704,7 +704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -727,7 +727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -750,7 +750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -773,7 +773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -796,7 +796,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -819,7 +819,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
@@ -827,7 +827,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -847,7 +847,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
         <v>57</v>
       </c>
@@ -870,16 +870,16 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="47.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -896,7 +896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -913,27 +913,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -954,13 +954,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.81640625" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -968,7 +968,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -976,7 +976,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -998,13 +998,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1053,12 +1053,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
ctf 2 & 9
</commit_message>
<xml_diff>
--- a/challenges.xlsx
+++ b/challenges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\twine-ctf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obakd\Documents\FH Wedel\IT-Sicherheit Projekt\twine-ctf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE7488D-77A0-4208-9DAF-FC533D73FB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EDC04F-B37C-4FF8-9E77-13385E4CB82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChallengesÜbersicht" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>ChallengeName</t>
   </si>
@@ -250,13 +250,19 @@
   </si>
   <si>
     <t xml:space="preserve">je nach bedarf können wir hier einen brief erstellen oder so </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lösung </t>
+  </si>
+  <si>
+    <t>picoCTF 2019 vault-door-1 Writeup – DMFR SECURITY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +289,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -324,10 +345,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -351,8 +373,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -390,9 +415,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:H19" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:H19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:I19" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ChallengeName"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nr. im Game"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Stufe" dataDxfId="0"/>
@@ -401,6 +426,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Typ"/>
     <tableColumn id="8" xr3:uid="{BE2C3356-256D-405E-BE1B-E0445F42102A}" name="simuliert"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Quelle"/>
+    <tableColumn id="9" xr3:uid="{E3D4471F-B0A3-476F-BF07-3E68248E5635}" name="Lösung "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -683,21 +709,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="79.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="79.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,8 +748,11 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -746,7 +775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -769,7 +798,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -792,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -815,7 +844,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -838,7 +867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -861,7 +890,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -884,7 +913,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -904,7 +933,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -923,8 +952,11 @@
       <c r="H10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -935,7 +967,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -960,10 +992,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I10" r:id="rId1" display="https://dmfrsecurity.com/2021/11/01/picoctf-2019-vault-door-1-writeup/" xr:uid="{6B6D9036-6650-419F-8539-D05D0655B5C8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -976,16 +1011,16 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="52.36328125" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1002,7 +1037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -1019,32 +1054,32 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1071,13 +1106,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.81640625" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1085,7 +1120,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1093,7 +1128,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1115,13 +1150,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1132,7 +1167,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1143,7 +1178,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1189,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1162,7 +1197,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1170,12 +1205,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
ctf6 start, storyline, ctf4-5 hints
</commit_message>
<xml_diff>
--- a/challenges.xlsx
+++ b/challenges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obakd\Documents\FH Wedel\IT-Sicherheit Projekt\twine-ctf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\uni_master\twine-ctf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B6D656-B667-4E5E-8733-21F2027467D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41DCF26-277A-49F7-9CA2-6AEFC761B66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChallengesÜbersicht" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="96">
   <si>
     <t>ChallengeName</t>
   </si>
@@ -194,12 +194,6 @@
     <t>look at js, base64 codiert user and pw</t>
   </si>
   <si>
-    <t xml:space="preserve">Same javascript funktion is executed </t>
-  </si>
-  <si>
-    <t>3*8-bit bytes is represented by four 6-bit digits with a particular set of 64 characters</t>
-  </si>
-  <si>
     <t>cft9</t>
   </si>
   <si>
@@ -300,6 +294,30 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Can you find a method that will be executed when you press the button?</t>
+  </si>
+  <si>
+    <t>What does the JavaScript funktion atob() do?</t>
+  </si>
+  <si>
+    <t>ctf5</t>
+  </si>
+  <si>
+    <t>ctf6</t>
+  </si>
+  <si>
+    <t>You need to insert some javascript, maybe the script tag helps</t>
+  </si>
+  <si>
+    <t>It is possible to pop an alert with javascript "alert()", you should only add some script-tags</t>
+  </si>
+  <si>
+    <t>Maybe there are other html tags that are vulnerable?</t>
+  </si>
+  <si>
+    <t>Think of an image tag, could you insert same javascript here (onerror= and src=)"</t>
   </si>
 </sst>
 </file>
@@ -393,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -419,7 +437,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -794,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -822,7 +839,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
@@ -834,13 +851,13 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -945,22 +962,22 @@
       <c r="C8" s="8">
         <v>1</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" t="s">
         <v>44</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="8">
         <v>2</v>
@@ -975,12 +992,12 @@
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
@@ -988,33 +1005,33 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>56</v>
+      <c r="E10" t="s">
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="8">
         <v>2</v>
@@ -1023,16 +1040,16 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
         <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1064,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1113,7 @@
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>52</v>
@@ -1105,52 +1122,74 @@
         <v>53</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>90</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1281,7 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DCD036-2CB5-4BFC-8E7C-2C6F414BD505}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1289,95 +1328,95 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
         <v>86</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files deleted and xlsx changed
</commit_message>
<xml_diff>
--- a/challenges.xlsx
+++ b/challenges.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\uni_master\twine-ctf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41DCF26-277A-49F7-9CA2-6AEFC761B66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95DC9D1-AEF7-4CA3-ACFE-89537A44402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32910" yWindow="2370" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChallengesÜbersicht" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="5" r:id="rId2"/>
-    <sheet name="Lösungen+Hints" sheetId="2" r:id="rId3"/>
-    <sheet name="Richtlinien" sheetId="3" r:id="rId4"/>
-    <sheet name="ToDos" sheetId="4" r:id="rId5"/>
-    <sheet name="Story Zuordnung" sheetId="6" r:id="rId6"/>
+    <sheet name="Lösungen+Hints" sheetId="2" r:id="rId2"/>
+    <sheet name="Richtlinien" sheetId="3" r:id="rId3"/>
+    <sheet name="ToDos" sheetId="4" r:id="rId4"/>
+    <sheet name="Story Zuordnung" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -411,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -437,6 +436,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +923,7 @@
         <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
         <v>39</v>
@@ -946,7 +946,7 @@
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>39</v>
@@ -982,10 +982,10 @@
       <c r="C9" s="8">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F9" t="s">
@@ -1066,22 +1066,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D365CF-5BE8-45C4-BEAB-B8E4702DC8BF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1194,7 +1182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1238,7 +1226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -1316,7 +1304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DCD036-2CB5-4BFC-8E7C-2C6F414BD505}">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>